<commit_message>
Testing setting files and reading calculated values
</commit_message>
<xml_diff>
--- a/test/dk/ative/docjure/testdata/simple.xlsx
+++ b/test/dk/ative/docjure/testdata/simple.xlsx
@@ -341,7 +341,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -367,6 +367,12 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <f>SUM(A2:B2)</f>
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>